<commit_message>
saving and updating graphs
</commit_message>
<xml_diff>
--- a/Data/Data_final.xlsx
+++ b/Data/Data_final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lolap\OneDrive\Documents\Cours\Master\MA2\Gaz Dissous\Code\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lolap\OneDrive\Documents\Cours\Master\MA2\Gaz Dissous\pyheadspace-main-final\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC285536-9883-42E2-A940-353DE342DB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBD131E-2185-478E-B357-B00DA7E6735C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -728,29 +728,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA33" sqref="AA33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" customWidth="1"/>
-    <col min="6" max="8" width="9.1796875" style="2"/>
-    <col min="9" max="9" width="19.90625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.81640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.26953125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="16.54296875" style="2" customWidth="1"/>
-    <col min="14" max="20" width="9.1796875" style="2"/>
-    <col min="21" max="21" width="15.1796875" style="2" customWidth="1"/>
-    <col min="22" max="22" width="9.1796875" style="2"/>
-    <col min="23" max="23" width="21.1796875" style="2" customWidth="1"/>
-    <col min="24" max="24" width="17.36328125" style="2" customWidth="1"/>
-    <col min="25" max="25" width="17.453125" customWidth="1"/>
-    <col min="26" max="26" width="20.81640625" customWidth="1"/>
-    <col min="27" max="27" width="18.6328125" customWidth="1"/>
-    <col min="28" max="28" width="18.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="1"/>
+    <col min="6" max="24" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -895,28 +880,28 @@
         <v>1016</v>
       </c>
       <c r="U2" s="2">
-        <v>1.4167817149999999</v>
+        <v>1.8335928860073889</v>
       </c>
       <c r="V2" s="2">
-        <v>425.18375889999999</v>
+        <v>433.83675948232349</v>
       </c>
       <c r="W2" s="2">
-        <v>1.5070706999999999E-2</v>
+        <v>-56.921563463333342</v>
       </c>
       <c r="X2" s="2">
-        <v>4.7185634719999996</v>
+        <v>-9.9155234024999999</v>
       </c>
       <c r="Y2">
-        <v>8.7986419531844492E-3</v>
+        <v>3.094426823591504E-3</v>
       </c>
       <c r="Z2">
-        <v>-172.69315132387109</v>
+        <v>-29.987497521374969</v>
       </c>
       <c r="AA2">
-        <v>17.010617044801119</v>
+        <v>16.892197529511328</v>
       </c>
       <c r="AB2">
-        <v>-17.005167178494538</v>
+        <v>-12.015240858390669</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.35">
@@ -975,28 +960,28 @@
         <v>1016</v>
       </c>
       <c r="U3" s="2">
-        <v>1.4167817149999999</v>
+        <v>1.8335928860073889</v>
       </c>
       <c r="V3" s="2">
-        <v>425.18375889999999</v>
+        <v>433.83675948232349</v>
       </c>
       <c r="W3" s="2">
-        <v>1.5070706999999999E-2</v>
+        <v>-56.921563463333342</v>
       </c>
       <c r="X3" s="2">
-        <v>4.7185634719999996</v>
+        <v>-9.9155234024999999</v>
       </c>
       <c r="Y3">
-        <v>6.8879478280648816E-3</v>
+        <v>1.183732698471937E-3</v>
       </c>
       <c r="Z3">
-        <v>-211.6228605855236</v>
+        <v>-26.61873100719248</v>
       </c>
       <c r="AA3">
-        <v>20.395721535975039</v>
+        <v>20.277302020685241</v>
       </c>
       <c r="AB3">
-        <v>-17.814917695776028</v>
+        <v>-13.662854633127999</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.35">
@@ -1061,22 +1046,22 @@
         <v>376.89630269999998</v>
       </c>
       <c r="W4" s="2">
-        <v>1.7946143000000001E-2</v>
+        <v>-54.962661850000003</v>
       </c>
       <c r="X4" s="2">
-        <v>4.2023151219999999</v>
+        <v>-10.123835120000001</v>
       </c>
       <c r="Y4">
         <v>4.3066027545636352E-3</v>
       </c>
       <c r="Z4">
-        <v>-363.7047473983144</v>
+        <v>-69.069968752057505</v>
       </c>
       <c r="AA4">
         <v>14.3678220560186</v>
       </c>
       <c r="AB4">
-        <v>-15.322786826926009</v>
+        <v>-10.170162418187131</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
@@ -1141,22 +1126,22 @@
         <v>376.89630269999998</v>
       </c>
       <c r="W5" s="2">
-        <v>1.7946143000000001E-2</v>
+        <v>-54.962661859999997</v>
       </c>
       <c r="X5" s="2">
-        <v>4.2023151219999999</v>
+        <v>-10.12383513</v>
       </c>
       <c r="Y5">
         <v>5.3111985677699236E-3</v>
       </c>
       <c r="Z5">
-        <v>-304.51422575346533</v>
+        <v>-65.442071932928386</v>
       </c>
       <c r="AA5">
         <v>14.534113502664461</v>
       </c>
       <c r="AB5">
-        <v>-11.257259096196901</v>
+        <v>-6.1631335093008666</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.35">
@@ -1221,22 +1206,22 @@
         <v>445.16345819999998</v>
       </c>
       <c r="W6" s="2">
-        <v>1.9807886E-2</v>
+        <v>-55.929852109999999</v>
       </c>
       <c r="X6" s="2">
-        <v>4.9584513340000003</v>
+        <v>-10.818008020000001</v>
       </c>
       <c r="Y6">
         <v>3.1393192049598779E-3</v>
       </c>
       <c r="Z6">
-        <v>-526.37736232246459</v>
+        <v>-74.970404126836982</v>
       </c>
       <c r="AA6">
         <v>13.034786724309869</v>
       </c>
       <c r="AB6">
-        <v>-15.798780107471041</v>
+        <v>-8.4469748773876585</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.35">
@@ -1301,22 +1286,22 @@
         <v>445.16345819999998</v>
       </c>
       <c r="W7" s="2">
-        <v>1.9807886E-2</v>
+        <v>-55.92985212</v>
       </c>
       <c r="X7" s="2">
-        <v>4.9584513340000003</v>
+        <v>-10.81800803</v>
       </c>
       <c r="Y7">
         <v>3.1665834200018629E-3</v>
       </c>
       <c r="Z7">
-        <v>-516.46073452013752</v>
+        <v>-68.860766056122785</v>
       </c>
       <c r="AA7">
         <v>13.70557189048021</v>
       </c>
       <c r="AB7">
-        <v>-12.306241382841311</v>
+        <v>-5.3137396892111166</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.35">
@@ -1381,22 +1366,22 @@
         <v>433.82134910000002</v>
       </c>
       <c r="W8" s="2">
-        <v>1.9892152999999999E-2</v>
+        <v>-54.967832059999999</v>
       </c>
       <c r="X8" s="2">
-        <v>4.8329789300000003</v>
+        <v>-10.432196769999999</v>
       </c>
       <c r="Y8">
         <v>2.160238126085596E-3</v>
       </c>
       <c r="Z8">
-        <v>-696.6256947843907</v>
+        <v>-53.879111877844778</v>
       </c>
       <c r="AA8">
         <v>13.28311124112029</v>
       </c>
       <c r="AB8">
-        <v>-14.45192617230939</v>
+        <v>-7.6804265916629033</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.35">
@@ -1461,22 +1446,22 @@
         <v>433.82134910000002</v>
       </c>
       <c r="W9" s="2">
-        <v>1.9892152999999999E-2</v>
+        <v>-54.96783207</v>
       </c>
       <c r="X9" s="2">
-        <v>4.8329789300000003</v>
+        <v>-10.43219678</v>
       </c>
       <c r="Y9">
         <v>2.5890625114570178E-3</v>
       </c>
       <c r="Z9">
-        <v>-610.53896915401879</v>
+        <v>-73.854208192095868</v>
       </c>
       <c r="AA9">
         <v>13.322440431540951</v>
       </c>
       <c r="AB9">
-        <v>-13.10754012315873</v>
+        <v>-6.3558314274152483</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.35">
@@ -1541,22 +1526,22 @@
         <v>435.53585579999998</v>
       </c>
       <c r="W10" s="2">
-        <v>1.9940528999999999E-2</v>
+        <v>-56.965777799999998</v>
       </c>
       <c r="X10" s="2">
-        <v>4.8534427239999998</v>
+        <v>-10.00010646</v>
       </c>
       <c r="Y10">
         <v>2.313060509072797E-3</v>
       </c>
       <c r="Z10">
-        <v>-709.55126793189174</v>
+        <v>-85.00562934969625</v>
       </c>
       <c r="AA10">
         <v>12.886240513395959</v>
       </c>
       <c r="AB10">
-        <v>-16.150672389329209</v>
+        <v>-9.3332575831532871</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.35">
@@ -1621,22 +1606,22 @@
         <v>435.53585579999998</v>
       </c>
       <c r="W11" s="2">
-        <v>1.9940528999999999E-2</v>
+        <v>-56.965777899999999</v>
       </c>
       <c r="X11" s="2">
-        <v>4.8534427239999998</v>
+        <v>-10.00010647</v>
       </c>
       <c r="Y11">
         <v>1.273072341096046E-3</v>
       </c>
       <c r="Z11">
-        <v>-1167.311000424859</v>
+        <v>-37.764903603325507</v>
       </c>
       <c r="AA11">
         <v>12.159238500098301</v>
       </c>
       <c r="AB11">
-        <v>-12.97942553951648</v>
+        <v>-5.7538575017105353</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.35">
@@ -1701,22 +1686,22 @@
         <v>425.93807659999999</v>
       </c>
       <c r="W12" s="2">
-        <v>1.9758871000000001E-2</v>
+        <v>-55.161032149999997</v>
       </c>
       <c r="X12" s="2">
-        <v>4.7511063609999997</v>
+        <v>-8.6518897119999991</v>
       </c>
       <c r="Y12">
         <v>1.9535766242476859E-3</v>
       </c>
       <c r="Z12">
-        <v>-757.69992928962938</v>
+        <v>-51.553582375473141</v>
       </c>
       <c r="AA12">
         <v>12.13082203666711</v>
       </c>
       <c r="AB12">
-        <v>-14.82722299042927</v>
+        <v>-8.4535109118620824</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.35">
@@ -1775,28 +1760,28 @@
         <v>1010.6</v>
       </c>
       <c r="U13" s="2">
-        <v>2.5673924170000002</v>
+        <v>1.8335928860073889</v>
       </c>
       <c r="V13" s="2">
-        <v>428.39231189999998</v>
+        <v>433.83675948232349</v>
       </c>
       <c r="W13" s="2">
-        <v>2.7385083000000001E-2</v>
+        <v>-56.921563463333342</v>
       </c>
       <c r="X13" s="2">
-        <v>4.772926827</v>
+        <v>-9.9155234024999999</v>
       </c>
       <c r="Y13">
-        <v>-7.0054080996426312E-3</v>
+        <v>2.906940855599578E-3</v>
       </c>
       <c r="Z13">
-        <v>214.0385215017366</v>
+        <v>-28.949042225207439</v>
       </c>
       <c r="AA13">
-        <v>12.49166138250607</v>
+        <v>12.41811641276275</v>
       </c>
       <c r="AB13">
-        <v>-14.02964905376802</v>
+        <v>-7.210428614838893</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.35">
@@ -1855,28 +1840,28 @@
         <v>1010.6</v>
       </c>
       <c r="U14" s="2">
-        <v>2.5673924170000002</v>
+        <v>1.8335928860073889</v>
       </c>
       <c r="V14" s="2">
-        <v>428.39231189999998</v>
+        <v>433.83675948232349</v>
       </c>
       <c r="W14" s="2">
-        <v>2.7385083000000001E-2</v>
+        <v>-56.921563463333342</v>
       </c>
       <c r="X14" s="2">
-        <v>4.772926827</v>
+        <v>-9.9155234024999999</v>
       </c>
       <c r="Y14">
-        <v>-7.6153841837834618E-3</v>
+        <v>2.296964771458747E-3</v>
       </c>
       <c r="Z14">
-        <v>197.37720473926319</v>
+        <v>-38.348758521608787</v>
       </c>
       <c r="AA14">
-        <v>14.04262998583361</v>
+        <v>13.96908501609029</v>
       </c>
       <c r="AB14">
-        <v>-16.120837409825729</v>
+        <v>-10.07008790525987</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.35">
@@ -1941,22 +1926,22 @@
         <v>401.94870529999997</v>
       </c>
       <c r="W15" s="2">
-        <v>1.9290706000000001E-2</v>
+        <v>-54.467110390000002</v>
       </c>
       <c r="X15" s="2">
-        <v>4.4780810070000001</v>
+        <v>-10.08089219</v>
       </c>
       <c r="Y15">
         <v>2.863116203685788E-3</v>
       </c>
       <c r="Z15">
-        <v>-523.37306033826292</v>
+        <v>-59.038431815159889</v>
       </c>
       <c r="AA15">
         <v>12.3656058813346</v>
       </c>
       <c r="AB15">
-        <v>-13.995303591023189</v>
+        <v>-7.5991324176979402</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.35">
@@ -2021,22 +2006,22 @@
         <v>401.94870529999997</v>
       </c>
       <c r="W16" s="2">
-        <v>1.9290706000000001E-2</v>
+        <v>-54.467110400000003</v>
       </c>
       <c r="X16" s="2">
-        <v>4.4780810070000001</v>
+        <v>-10.080892199999999</v>
       </c>
       <c r="Y16">
         <v>3.4724421673064249E-3</v>
       </c>
       <c r="Z16">
-        <v>-454.50987994894251</v>
+        <v>-71.413519203312731</v>
       </c>
       <c r="AA16">
         <v>12.824036640454979</v>
       </c>
       <c r="AB16">
-        <v>-12.798178964173349</v>
+        <v>-6.6305089607735512</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.35">
@@ -2101,22 +2086,22 @@
         <v>426.38456079999997</v>
       </c>
       <c r="W17" s="2">
-        <v>1.9630239000000001E-2</v>
+        <v>-55.223878399999997</v>
       </c>
       <c r="X17" s="2">
-        <v>4.7509650990000001</v>
+        <v>-9.9718146890000003</v>
       </c>
       <c r="Y17">
         <v>2.6463650133031428E-3</v>
       </c>
       <c r="Z17">
-        <v>-587.03370068996821</v>
+        <v>-67.508858249188066</v>
       </c>
       <c r="AA17">
         <v>12.60328512536244</v>
       </c>
       <c r="AB17">
-        <v>-14.084294278279289</v>
+        <v>-7.3366356704104296</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.35">
@@ -2181,22 +2166,22 @@
         <v>426.38456079999997</v>
       </c>
       <c r="W18" s="2">
-        <v>1.9630239000000001E-2</v>
+        <v>-55.223878499999998</v>
       </c>
       <c r="X18" s="2">
-        <v>4.7509650990000001</v>
+        <v>-9.9718146900000004</v>
       </c>
       <c r="Y18">
         <v>2.80671947978549E-3</v>
       </c>
       <c r="Z18">
-        <v>-550.11778978465475</v>
+        <v>-60.032839705966737</v>
       </c>
       <c r="AA18">
         <v>13.08850982013441</v>
       </c>
       <c r="AB18">
-        <v>-12.48949881771278</v>
+        <v>-5.9917820421501178</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.35">
@@ -2261,22 +2246,22 @@
         <v>434.12229908788203</v>
       </c>
       <c r="W19" s="2">
-        <v>1.96930436347586E-2</v>
+        <v>-57.196125119999998</v>
       </c>
       <c r="X19" s="2">
-        <v>4.8421454403630504</v>
+        <v>-9.0503898150000008</v>
       </c>
       <c r="Y19">
         <v>2.6672394797877682E-3</v>
       </c>
       <c r="Z19">
-        <v>-578.80778892268859</v>
+        <v>-43.638872427387398</v>
       </c>
       <c r="AA19">
         <v>11.78628813985136</v>
       </c>
       <c r="AB19">
-        <v>-13.778550185778011</v>
+        <v>-6.8687693718824114</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.35">
@@ -2341,22 +2326,22 @@
         <v>434.12229908788203</v>
       </c>
       <c r="W20" s="2">
-        <v>1.96930436347586E-2</v>
+        <v>-57.196125129999999</v>
       </c>
       <c r="X20" s="2">
-        <v>4.8421454403630504</v>
+        <v>-9.0503898159999991</v>
       </c>
       <c r="Y20">
         <v>1.0753179297020439E-2</v>
       </c>
       <c r="Z20">
-        <v>-167.9098347095055</v>
+        <v>-34.54512387817099</v>
       </c>
       <c r="AA20">
         <v>12.209154891068099</v>
       </c>
       <c r="AB20">
-        <v>-13.27394907325175</v>
+        <v>-6.6034332372819637</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.35">
@@ -2421,22 +2406,22 @@
         <v>453.20552079999999</v>
       </c>
       <c r="W21" s="2">
-        <v>1.9627262999999999E-2</v>
+        <v>-59.204145969999999</v>
       </c>
       <c r="X21" s="2">
-        <v>5.0453170900000002</v>
+        <v>-10.972126019999999</v>
       </c>
       <c r="Y21">
         <v>2.5083802070741731E-3</v>
       </c>
       <c r="Z21">
-        <v>-601.338345220664</v>
+        <v>-14.28188532058727</v>
       </c>
       <c r="AA21">
         <v>12.40460381902483</v>
       </c>
       <c r="AB21">
-        <v>-14.444606292561829</v>
+        <v>-6.5599045270557932</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.35">
@@ -2501,22 +2486,22 @@
         <v>453.20552079999999</v>
       </c>
       <c r="W22" s="2">
-        <v>1.9627262999999999E-2</v>
+        <v>-59.20414598</v>
       </c>
       <c r="X22" s="2">
-        <v>5.0453170900000002</v>
+        <v>-10.97212603</v>
       </c>
       <c r="Y22">
         <v>2.6246246810573831E-3</v>
       </c>
       <c r="Z22">
-        <v>-609.79545738422769</v>
+        <v>-49.007939392600399</v>
       </c>
       <c r="AA22">
         <v>13.692604486263971</v>
       </c>
       <c r="AB22">
-        <v>-15.64113485090213</v>
+        <v>-8.4983585245748117</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.35">
@@ -2581,22 +2566,22 @@
         <v>453.20552079999999</v>
       </c>
       <c r="W23" s="2">
-        <v>1.9627262999999999E-2</v>
+        <v>-59.204145990000001</v>
       </c>
       <c r="X23" s="2">
-        <v>5.0453170900000002</v>
+        <v>-10.972126039999999</v>
       </c>
       <c r="Y23">
         <v>1.7903520265769349E-3</v>
       </c>
       <c r="Z23">
-        <v>-888.02078988385836</v>
+        <v>-68.640258916474735</v>
       </c>
       <c r="AA23">
         <v>13.11377210512663</v>
       </c>
       <c r="AB23">
-        <v>-13.42681453214178</v>
+        <v>-5.9683699643656718</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.35">
@@ -2661,22 +2646,22 @@
         <v>461.01353599999999</v>
       </c>
       <c r="W24" s="2">
-        <v>1.9088435000000001E-2</v>
+        <v>-61.177933860000003</v>
       </c>
       <c r="X24" s="2">
-        <v>5.1437586780000002</v>
+        <v>-9.1076751859999998</v>
       </c>
       <c r="Y24">
         <v>3.8477303472249391E-3</v>
       </c>
       <c r="Z24">
-        <v>-409.09747965269941</v>
+        <v>-23.059563032512109</v>
       </c>
       <c r="AA24">
         <v>12.308226243219529</v>
       </c>
       <c r="AB24">
-        <v>-16.3167790810067</v>
+        <v>-9.1283280135923128</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.35">
@@ -2741,22 +2726,22 @@
         <v>451.92330140000001</v>
       </c>
       <c r="W25" s="2">
-        <v>1.8959759999999999E-2</v>
+        <v>-60.025576095000012</v>
       </c>
       <c r="X25" s="2">
-        <v>5.0397000790000002</v>
+        <v>-9.5691955029999995</v>
       </c>
       <c r="Y25">
         <v>3.3479402018581602E-3</v>
       </c>
       <c r="Z25">
-        <v>-436.14731047713133</v>
+        <v>-5.5429259398406261</v>
       </c>
       <c r="AA25">
         <v>12.204093082609891</v>
       </c>
       <c r="AB25">
-        <v>-14.357927366915099</v>
+        <v>-7.0926381981493147</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.35">
@@ -2821,22 +2806,22 @@
         <v>451.92330140000001</v>
       </c>
       <c r="W26" s="2">
-        <v>1.8959759999999999E-2</v>
+        <v>-60.025576095000012</v>
       </c>
       <c r="X26" s="2">
-        <v>5.0397000790000002</v>
+        <v>-9.5691955029999995</v>
       </c>
       <c r="Y26">
         <v>3.8534761595845741E-3</v>
       </c>
       <c r="Z26">
-        <v>-412.93589801849299</v>
+        <v>-38.863721562419457</v>
       </c>
       <c r="AA26">
         <v>12.58057404693619</v>
       </c>
       <c r="AB26">
-        <v>-12.52443539377601</v>
+        <v>-5.4762953462041963</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.35">
@@ -2901,22 +2886,22 @@
         <v>442.83306679999998</v>
       </c>
       <c r="W27" s="2">
-        <v>1.8831085000000001E-2</v>
+        <v>-58.87321833</v>
       </c>
       <c r="X27" s="2">
-        <v>4.9356414800000001</v>
+        <v>-10.030715819999999</v>
       </c>
       <c r="Y27">
         <v>2.1392763993178989E-3</v>
       </c>
       <c r="Z27">
-        <v>-685.58456005589005</v>
+        <v>-34.329058174857757</v>
       </c>
       <c r="AA27">
         <v>15.10032076708951</v>
       </c>
       <c r="AB27">
-        <v>-16.85754820523999</v>
+        <v>-10.984821800440249</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.35">
@@ -2981,22 +2966,22 @@
         <v>469.17838260000002</v>
       </c>
       <c r="W28" s="2">
-        <v>1.9672393999999999E-2</v>
+        <v>-58.929193519999998</v>
       </c>
       <c r="X28" s="2">
-        <v>5.2293654299999996</v>
+        <v>-9.7466310279999995</v>
       </c>
       <c r="Y28">
         <v>2.6723683008303312E-3</v>
       </c>
       <c r="Z28">
-        <v>-589.52349097971648</v>
+        <v>-41.973387098349633</v>
       </c>
       <c r="AA28">
         <v>14.04731950972567</v>
       </c>
       <c r="AB28">
-        <v>-14.31528922837211</v>
+        <v>-7.5997118670074748</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.35">
@@ -3061,22 +3046,22 @@
         <v>469.17838260000002</v>
       </c>
       <c r="W29" s="2">
-        <v>1.9672393999999999E-2</v>
+        <v>-58.929193529999999</v>
       </c>
       <c r="X29" s="2">
-        <v>5.2293654299999996</v>
+        <v>-9.7466310289999996</v>
       </c>
       <c r="Y29">
         <v>2.756504072801392E-3</v>
       </c>
       <c r="Z29">
-        <v>-559.06956582865462</v>
+        <v>-27.969964685378159</v>
       </c>
       <c r="AA29">
         <v>14.374101905881639</v>
       </c>
       <c r="AB29">
-        <v>-14.022191817537831</v>
+        <v>-7.4592556575592273</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.35">
@@ -3141,22 +3126,22 @@
         <v>428.6505975</v>
       </c>
       <c r="W30" s="2">
-        <v>2.0263805999999999E-2</v>
+        <v>-53.667842299999997</v>
       </c>
       <c r="X30" s="2">
-        <v>4.7792168410000002</v>
+        <v>-9.4657855190000006</v>
       </c>
       <c r="Y30">
         <v>4.148862416880339E-3</v>
       </c>
       <c r="Z30">
-        <v>-415.20836405210929</v>
+        <v>-64.572766706793345</v>
       </c>
       <c r="AA30">
         <v>15.86042245163045</v>
       </c>
       <c r="AB30">
-        <v>-13.199130987740171</v>
+        <v>-7.6997745456384159</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.35">
@@ -3221,22 +3206,22 @@
         <v>428.6505975</v>
       </c>
       <c r="W31" s="2">
-        <v>2.0263805999999999E-2</v>
+        <v>-53.667842399999998</v>
       </c>
       <c r="X31" s="2">
-        <v>4.7792168410000002</v>
+        <v>-9.4657855200000007</v>
       </c>
       <c r="Y31">
         <v>4.2777133855035647E-3</v>
       </c>
       <c r="Z31">
-        <v>-401.87961289636598</v>
+        <v>-61.744679774671908</v>
       </c>
       <c r="AA31">
         <v>15.48953659619592</v>
       </c>
       <c r="AB31">
-        <v>-11.582660149749071</v>
+        <v>-5.95141603735172</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.35">
@@ -3301,22 +3286,22 @@
         <v>409.18969220000002</v>
       </c>
       <c r="W32" s="2">
-        <v>1.9294425E-2</v>
+        <v>-52.742472229999997</v>
       </c>
       <c r="X32" s="2">
-        <v>4.564363502</v>
+        <v>-8.9464004369999994</v>
       </c>
       <c r="Y32">
         <v>1.8840000798497809E-2</v>
       </c>
       <c r="Z32">
-        <v>-139.31512409245701</v>
+        <v>-66.805941919899297</v>
       </c>
       <c r="AA32">
         <v>17.63643212185108</v>
       </c>
       <c r="AB32">
-        <v>-13.338908974866889</v>
+        <v>-8.8546116854044676</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.35">
@@ -3381,22 +3366,22 @@
         <v>409.18969220000002</v>
       </c>
       <c r="W33" s="2">
-        <v>1.9294425E-2</v>
+        <v>-52.742472239999998</v>
       </c>
       <c r="X33" s="2">
-        <v>4.564363502</v>
+        <v>-8.9464004379999995</v>
       </c>
       <c r="Y33">
         <v>5.0992767757006554E-3</v>
       </c>
       <c r="Z33">
-        <v>-338.2930720208185</v>
+        <v>-71.000310513008586</v>
       </c>
       <c r="AA33">
         <v>16.76261546046538</v>
       </c>
       <c r="AB33">
-        <v>-11.385024651412889</v>
+        <v>-6.6667498028916139</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.35">
@@ -3461,22 +3446,22 @@
         <v>425.92079680000001</v>
       </c>
       <c r="W34" s="2">
-        <v>2.0400456000000001E-2</v>
+        <v>-54.481109349999997</v>
       </c>
       <c r="X34" s="2">
-        <v>4.7503374010000003</v>
+        <v>-8.9611472350000003</v>
       </c>
       <c r="Y34">
         <v>9.2946502253593176E-4</v>
       </c>
       <c r="Z34">
-        <v>-1630.653147127696</v>
+        <v>-53.572785691703317</v>
       </c>
       <c r="AA34">
         <v>15.84829761573134</v>
       </c>
       <c r="AB34">
-        <v>-12.575465815604311</v>
+        <v>-7.3198999362500414</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.35">
@@ -3541,22 +3526,22 @@
         <v>425.92079680000001</v>
       </c>
       <c r="W35" s="2">
-        <v>2.0400456000000001E-2</v>
+        <v>-54.481109359999998</v>
       </c>
       <c r="X35" s="2">
-        <v>4.7503374010000003</v>
+        <v>-8.9611472360000004</v>
       </c>
       <c r="Y35">
         <v>3.9362051165427398E-3</v>
       </c>
       <c r="Z35">
-        <v>-438.97234523744521</v>
+        <v>-61.609548827279312</v>
       </c>
       <c r="AA35">
         <v>17.12329872440429</v>
       </c>
       <c r="AB35">
-        <v>-12.05689641067187</v>
+        <v>-7.1926253148590913</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.35">
@@ -3621,22 +3606,22 @@
         <v>431.67977839999998</v>
       </c>
       <c r="W36" s="2">
-        <v>2.0250593000000001E-2</v>
+        <v>-55.749257299999996</v>
       </c>
       <c r="X36" s="2">
-        <v>4.8151137110000004</v>
+        <v>-8.8215445740000007</v>
       </c>
       <c r="Y36">
         <v>3.0632763796748512E-3</v>
       </c>
       <c r="Z36">
-        <v>-530.78580818635874</v>
+        <v>-40.815159054814373</v>
       </c>
       <c r="AA36">
         <v>17.357286913651048</v>
       </c>
       <c r="AB36">
-        <v>-12.52834722807361</v>
+        <v>-7.7192718634748747</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.35">
@@ -3701,22 +3686,22 @@
         <v>431.67977839999998</v>
       </c>
       <c r="W37" s="2">
-        <v>2.0250593000000001E-2</v>
+        <v>-55.749257399999998</v>
       </c>
       <c r="X37" s="2">
-        <v>4.8151137110000004</v>
+        <v>-8.8215445750000008</v>
       </c>
       <c r="Y37">
         <v>3.771834849239139E-3</v>
       </c>
       <c r="Z37">
-        <v>-446.76102079645409</v>
+        <v>-48.49583572837868</v>
       </c>
       <c r="AA37">
         <v>17.102070870687509</v>
       </c>
       <c r="AB37">
-        <v>-12.26154795759704</v>
+        <v>-7.3806735695958192</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.35">
@@ -3781,22 +3766,22 @@
         <v>430.28705200000002</v>
       </c>
       <c r="W38" s="2">
-        <v>2.0259525E-2</v>
+        <v>-55.278645619999999</v>
       </c>
       <c r="X38" s="2">
-        <v>4.7999479550000004</v>
+        <v>-8.7287765089999994</v>
       </c>
       <c r="Y38">
         <v>3.7435667598590639E-3</v>
       </c>
       <c r="Z38">
-        <v>-464.40417120133822</v>
+        <v>-56.778306121441638</v>
       </c>
       <c r="AA38">
         <v>20.76062096472975</v>
       </c>
       <c r="AB38">
-        <v>-12.351565812834361</v>
+        <v>-8.2768159256720875</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.35">
@@ -3861,22 +3846,22 @@
         <v>430.28705200000002</v>
       </c>
       <c r="W39" s="2">
-        <v>2.0259525E-2</v>
+        <v>-55.27864563</v>
       </c>
       <c r="X39" s="2">
-        <v>4.7999479550000004</v>
+        <v>-8.7287765099999994</v>
       </c>
       <c r="Y39">
         <v>4.6316177526309031E-3</v>
       </c>
       <c r="Z39">
-        <v>-435.67231818330612</v>
+        <v>-106.2785673972506</v>
       </c>
       <c r="AA39">
         <v>22.11925578610898</v>
       </c>
       <c r="AB39">
-        <v>-13.653503092230119</v>
+        <v>-9.8291579695037878</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.35">
@@ -3941,22 +3926,22 @@
         <v>425.33562430000001</v>
       </c>
       <c r="W40" s="2">
-        <v>2.0131275000000001E-2</v>
+        <v>-52.67334237</v>
       </c>
       <c r="X40" s="2">
-        <v>4.746710996</v>
+        <v>-8.270844147</v>
       </c>
       <c r="Y40">
         <v>4.0924759749951106E-3</v>
       </c>
       <c r="Z40">
-        <v>-407.20916575577428</v>
+        <v>-61.070568130434211</v>
       </c>
       <c r="AA40">
         <v>17.982750875783282</v>
       </c>
       <c r="AB40">
-        <v>-11.76180466632737</v>
+        <v>-7.3654144031187752</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.35">
@@ -4021,22 +4006,22 @@
         <v>425.33562430000001</v>
       </c>
       <c r="W41" s="2">
-        <v>2.0131275000000001E-2</v>
+        <v>-52.673342380000001</v>
       </c>
       <c r="X41" s="2">
-        <v>4.746710996</v>
+        <v>-8.2708441480000001</v>
       </c>
       <c r="Y41">
         <v>4.4255615867307861E-3</v>
       </c>
       <c r="Z41">
-        <v>-409.22465451192312</v>
+        <v>-89.244784328176621</v>
       </c>
       <c r="AA41">
         <v>19.695014769314671</v>
       </c>
       <c r="AB41">
-        <v>-12.08349086415217</v>
+        <v>-8.0693636766269172</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.35">
@@ -4101,22 +4086,22 @@
         <v>435.60845430000001</v>
       </c>
       <c r="W42" s="2">
-        <v>2.0122201999999999E-2</v>
+        <v>-56.098485160000003</v>
       </c>
       <c r="X42" s="2">
-        <v>4.85986911</v>
+        <v>-8.5428013939999996</v>
       </c>
       <c r="Y42">
         <v>3.737855902050986E-3</v>
       </c>
       <c r="Z42">
-        <v>-441.68506239189969</v>
+        <v>-33.864673745682254</v>
       </c>
       <c r="AA42">
         <v>17.285677661063509</v>
       </c>
       <c r="AB42">
-        <v>-12.404645600412881</v>
+        <v>-7.5468825675604201</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.35">
@@ -4181,22 +4166,22 @@
         <v>421.04738659999998</v>
       </c>
       <c r="W43" s="2">
-        <v>2.0530521999999999E-2</v>
+        <v>-53.996053099999997</v>
       </c>
       <c r="X43" s="2">
-        <v>4.697638091</v>
+        <v>-8.4924573149999993</v>
       </c>
       <c r="Y43">
         <v>3.241542899826721E-3</v>
       </c>
       <c r="Z43">
-        <v>-530.52884053095875</v>
+        <v>-68.350281365530122</v>
       </c>
       <c r="AA43">
         <v>18.442427830026219</v>
       </c>
       <c r="AB43">
-        <v>-12.362243672793481</v>
+        <v>-8.0122280938587096</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.35">
@@ -4261,22 +4246,22 @@
         <v>421.04738659999998</v>
       </c>
       <c r="W44" s="2">
-        <v>2.0530521999999999E-2</v>
+        <v>-53.996053199999999</v>
       </c>
       <c r="X44" s="2">
-        <v>4.697638091</v>
+        <v>-8.4924573159999994</v>
       </c>
       <c r="Y44">
         <v>3.813010751166889E-3</v>
       </c>
       <c r="Z44">
-        <v>-475.73028712429738</v>
+        <v>-82.64258495025156</v>
       </c>
       <c r="AA44">
         <v>18.87583009965714</v>
       </c>
       <c r="AB44">
-        <v>-12.517394472345339</v>
+        <v>-8.2672775733730894</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.35">
@@ -4341,22 +4326,22 @@
         <v>439.51656709999997</v>
       </c>
       <c r="W45" s="2">
-        <v>1.8623842000000002E-2</v>
+        <v>-66.0492414</v>
       </c>
       <c r="X45" s="2">
-        <v>4.8954792920000001</v>
+        <v>-10.205312859999999</v>
       </c>
       <c r="Y45">
         <v>4.7286491734834296E-3</v>
       </c>
       <c r="Z45">
-        <v>-336.55235322592171</v>
+        <v>16.20471131516199</v>
       </c>
       <c r="AA45">
         <v>15.685560010365799</v>
       </c>
       <c r="AB45">
-        <v>-16.966578994914052</v>
+        <v>-10.930904350645919</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.35">
@@ -4421,22 +4406,22 @@
         <v>439.51656709999997</v>
       </c>
       <c r="W46" s="2">
-        <v>1.8623842000000002E-2</v>
+        <v>-66.049241499999994</v>
       </c>
       <c r="X46" s="2">
-        <v>4.8954792920000001</v>
+        <v>-10.20531287</v>
       </c>
       <c r="Y46">
         <v>6.3784988907145072E-3</v>
       </c>
       <c r="Z46">
-        <v>-307.51824463172051</v>
+        <v>-46.100527736909306</v>
       </c>
       <c r="AA46">
         <v>18.481401824916212</v>
       </c>
       <c r="AB46">
-        <v>-13.06309392816285</v>
+        <v>-7.9400975374979144</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.35">
@@ -4501,22 +4486,22 @@
         <v>418.20489129999999</v>
       </c>
       <c r="W47" s="2">
-        <v>2.0140565999999999E-2</v>
+        <v>-55.302911600000002</v>
       </c>
       <c r="X47" s="2">
-        <v>4.6664406730000003</v>
+        <v>-8.3687344899999996</v>
       </c>
       <c r="Y47">
         <v>4.6148251241909122E-3</v>
       </c>
       <c r="Z47">
-        <v>-394.50341015363938</v>
+        <v>-67.222141792508296</v>
       </c>
       <c r="AA47">
         <v>20.797618564580009</v>
       </c>
       <c r="AB47">
-        <v>-12.09705734870237</v>
+        <v>-8.3089935587127286</v>
       </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.35">
@@ -4581,22 +4566,22 @@
         <v>421.55145099999999</v>
       </c>
       <c r="W48" s="2">
-        <v>2.0412426000000001E-2</v>
+        <v>-57.020228019999998</v>
       </c>
       <c r="X48" s="2">
-        <v>4.7042345900000004</v>
+        <v>-8.2502803119999992</v>
       </c>
       <c r="Y48">
         <v>5.0843408975148503E-3</v>
       </c>
       <c r="Z48">
-        <v>-387.11285517596082</v>
+        <v>-77.182936164740596</v>
       </c>
       <c r="AA48">
         <v>22.12089005090899</v>
       </c>
       <c r="AB48">
-        <v>-12.69580671896264</v>
+        <v>-9.1401420243376599</v>
       </c>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.35">
@@ -4661,22 +4646,22 @@
         <v>421.55145099999999</v>
       </c>
       <c r="W49" s="2">
-        <v>2.0412426000000001E-2</v>
+        <v>-57.020228029999998</v>
       </c>
       <c r="X49" s="2">
-        <v>4.7042345900000004</v>
+        <v>-8.2502803129999993</v>
       </c>
       <c r="Y49">
         <v>5.5082743457000724E-3</v>
       </c>
       <c r="Z49">
-        <v>-361.95988315819449</v>
+        <v>-75.798823143129241</v>
       </c>
       <c r="AA49">
         <v>21.029784370028359</v>
       </c>
       <c r="AB49">
-        <v>-12.48314303175246</v>
+        <v>-8.742971625631867</v>
       </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.35">
@@ -4741,22 +4726,22 @@
         <v>419.37594689999997</v>
       </c>
       <c r="W50" s="2">
-        <v>2.0358905E-2</v>
+        <v>-55.807492770000003</v>
       </c>
       <c r="X50" s="2">
-        <v>4.6778208269999997</v>
+        <v>-8.6970304479999996</v>
       </c>
       <c r="Y50">
         <v>4.2413462417942843E-3</v>
       </c>
       <c r="Z50">
-        <v>-415.48085690849848</v>
+        <v>-53.438936396761562</v>
       </c>
       <c r="AA50">
         <v>21.51911591464194</v>
       </c>
       <c r="AB50">
-        <v>-11.988972053983529</v>
+        <v>-8.2361804841000197</v>
       </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.35">
@@ -4821,22 +4806,22 @@
         <v>421.86555570000002</v>
       </c>
       <c r="W51" s="2">
-        <v>1.9631084E-2</v>
+        <v>-56.159641149999999</v>
       </c>
       <c r="X51" s="2">
-        <v>4.7064091809999997</v>
+        <v>-8.5407833879999995</v>
       </c>
       <c r="Y51">
         <v>5.7365590205784803E-3</v>
       </c>
       <c r="Z51">
-        <v>-319.52677600546639</v>
+        <v>-61.391920609061287</v>
       </c>
       <c r="AA51">
         <v>22.438140294355399</v>
       </c>
       <c r="AB51">
-        <v>-12.534074487830059</v>
+        <v>-8.9751160578809284</v>
       </c>
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.35">
@@ -4901,22 +4886,22 @@
         <v>421.86555570000002</v>
       </c>
       <c r="W52" s="2">
-        <v>1.9631084E-2</v>
+        <v>-56.15964116</v>
       </c>
       <c r="X52" s="2">
-        <v>4.7064091809999997</v>
+        <v>-8.5407833889999996</v>
       </c>
       <c r="Y52">
         <v>5.3963960558856454E-3</v>
       </c>
       <c r="Z52">
-        <v>-336.90103212351909</v>
+        <v>-62.551010307907113</v>
       </c>
       <c r="AA52">
         <v>21.674671631048842</v>
       </c>
       <c r="AB52">
-        <v>-11.87215119117824</v>
+        <v>-8.187772959868056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>